<commit_message>
results, sped up algorithm a bit
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fax\job_shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4845FC0-10CC-4C1D-A5C3-8177868BC06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C67A24-CFA5-42E5-AA68-72EFADA87BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{578F53E5-FEB2-48EB-9BE3-4B9F2C470EAD}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Best known</t>
   </si>
   <si>
-    <t>Best</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>LA35</t>
+  </si>
+  <si>
+    <t>Best Achieved</t>
   </si>
 </sst>
 </file>
@@ -516,12 +516,13 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -559,10 +560,10 @@
         <v>5</v>
       </c>
       <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
         <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -606,7 +607,7 @@
         <v>55</v>
       </c>
       <c r="O2">
-        <f>AVERAGE(B2:K2)</f>
+        <f t="shared" ref="O2:O12" si="0">AVERAGE(B2:K2)</f>
         <v>55.4</v>
       </c>
     </row>
@@ -651,7 +652,7 @@
         <v>960</v>
       </c>
       <c r="O3">
-        <f>AVERAGE(B3:K3)</f>
+        <f t="shared" si="0"/>
         <v>1017.9</v>
       </c>
     </row>
@@ -684,10 +685,10 @@
         <v>1314</v>
       </c>
       <c r="J4">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="K4">
-        <v>1333</v>
+        <v>1323</v>
       </c>
       <c r="M4">
         <v>1165</v>
@@ -696,8 +697,8 @@
         <v>1260</v>
       </c>
       <c r="O4">
-        <f>AVERAGE(B4:K4)</f>
-        <v>1310.0999999999999</v>
+        <f t="shared" si="0"/>
+        <v>1308.7</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -741,13 +742,13 @@
         <v>666</v>
       </c>
       <c r="O5">
-        <f>AVERAGE(B5:K5)</f>
+        <f t="shared" si="0"/>
         <v>666.2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>689</v>
@@ -758,21 +759,86 @@
       <c r="D6">
         <v>709</v>
       </c>
+      <c r="E6">
+        <v>705</v>
+      </c>
+      <c r="F6">
+        <v>682</v>
+      </c>
+      <c r="G6">
+        <v>703</v>
+      </c>
+      <c r="H6">
+        <v>700</v>
+      </c>
+      <c r="I6">
+        <v>709</v>
+      </c>
+      <c r="J6">
+        <v>701</v>
+      </c>
+      <c r="K6">
+        <v>685</v>
+      </c>
       <c r="M6">
         <v>655</v>
       </c>
+      <c r="N6">
+        <v>682</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>699.3</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>622</v>
+      </c>
+      <c r="C7">
+        <v>627</v>
+      </c>
+      <c r="D7">
+        <v>621</v>
+      </c>
+      <c r="E7">
+        <v>641</v>
+      </c>
+      <c r="F7">
+        <v>628</v>
+      </c>
+      <c r="G7">
+        <v>619</v>
+      </c>
+      <c r="H7">
+        <v>632</v>
+      </c>
+      <c r="I7">
+        <v>622</v>
+      </c>
+      <c r="J7">
+        <v>630</v>
+      </c>
+      <c r="K7">
+        <v>619</v>
       </c>
       <c r="M7">
         <v>597</v>
       </c>
+      <c r="N7">
+        <v>619</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>626.1</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>611</v>
@@ -780,270 +846,1473 @@
       <c r="C8">
         <v>614</v>
       </c>
+      <c r="D8">
+        <v>611</v>
+      </c>
+      <c r="E8">
+        <v>619</v>
+      </c>
+      <c r="F8">
+        <v>611</v>
+      </c>
+      <c r="G8">
+        <v>616</v>
+      </c>
+      <c r="H8">
+        <v>611</v>
+      </c>
+      <c r="I8">
+        <v>611</v>
+      </c>
+      <c r="J8">
+        <v>611</v>
+      </c>
+      <c r="K8">
+        <v>611</v>
+      </c>
       <c r="M8">
         <v>590</v>
       </c>
+      <c r="N8">
+        <v>611</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>612.6</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>593</v>
+      </c>
+      <c r="C9">
+        <v>593</v>
+      </c>
+      <c r="D9">
+        <v>593</v>
+      </c>
+      <c r="E9">
+        <v>593</v>
+      </c>
+      <c r="F9">
+        <v>593</v>
+      </c>
+      <c r="G9">
+        <v>593</v>
+      </c>
+      <c r="H9">
+        <v>593</v>
+      </c>
+      <c r="I9">
+        <v>593</v>
+      </c>
+      <c r="J9">
+        <v>593</v>
+      </c>
+      <c r="K9">
+        <v>593</v>
       </c>
       <c r="M9">
         <v>593</v>
       </c>
+      <c r="N9">
+        <v>593</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>593</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>926</v>
+      </c>
+      <c r="C10">
+        <v>926</v>
+      </c>
+      <c r="D10">
+        <v>926</v>
+      </c>
+      <c r="E10">
+        <v>926</v>
+      </c>
+      <c r="F10">
+        <v>926</v>
+      </c>
+      <c r="G10">
+        <v>926</v>
+      </c>
+      <c r="H10">
+        <v>926</v>
+      </c>
+      <c r="I10">
+        <v>926</v>
+      </c>
+      <c r="J10">
+        <v>926</v>
+      </c>
+      <c r="K10">
+        <v>926</v>
       </c>
       <c r="M10">
         <v>926</v>
       </c>
+      <c r="N10">
+        <v>926</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>926</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>890</v>
+      </c>
+      <c r="C11">
+        <v>892</v>
+      </c>
+      <c r="D11">
+        <v>890</v>
+      </c>
+      <c r="E11">
+        <v>910</v>
+      </c>
+      <c r="F11">
+        <v>905</v>
+      </c>
+      <c r="G11">
+        <v>890</v>
+      </c>
+      <c r="H11">
+        <v>902</v>
+      </c>
+      <c r="I11">
+        <v>890</v>
+      </c>
+      <c r="J11">
+        <v>895</v>
+      </c>
+      <c r="K11">
+        <v>890</v>
       </c>
       <c r="M11">
         <v>890</v>
       </c>
+      <c r="N11">
+        <v>890</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>895.4</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>863</v>
+      </c>
+      <c r="C12">
+        <v>863</v>
+      </c>
+      <c r="D12">
+        <v>863</v>
+      </c>
+      <c r="E12">
+        <v>863</v>
+      </c>
+      <c r="F12">
+        <v>863</v>
+      </c>
+      <c r="G12">
+        <v>863</v>
+      </c>
+      <c r="H12">
+        <v>863</v>
+      </c>
+      <c r="I12">
+        <v>863</v>
+      </c>
+      <c r="J12">
+        <v>863</v>
+      </c>
+      <c r="K12">
+        <v>863</v>
       </c>
       <c r="M12">
         <v>863</v>
       </c>
+      <c r="N12">
+        <v>863</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>863</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>951</v>
+      </c>
+      <c r="C13">
+        <v>951</v>
+      </c>
+      <c r="D13">
+        <v>951</v>
+      </c>
+      <c r="E13">
+        <v>951</v>
+      </c>
+      <c r="F13">
+        <v>951</v>
+      </c>
+      <c r="G13">
+        <v>951</v>
+      </c>
+      <c r="H13">
+        <v>951</v>
+      </c>
+      <c r="I13">
+        <v>951</v>
+      </c>
+      <c r="J13">
+        <v>951</v>
+      </c>
+      <c r="K13">
+        <v>951</v>
       </c>
       <c r="M13">
         <v>951</v>
       </c>
+      <c r="N13">
+        <v>951</v>
+      </c>
+      <c r="O13">
+        <v>951</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>958</v>
+      </c>
+      <c r="C14">
+        <v>958</v>
+      </c>
+      <c r="D14">
+        <v>958</v>
+      </c>
+      <c r="E14">
+        <v>958</v>
+      </c>
+      <c r="F14">
+        <v>958</v>
+      </c>
+      <c r="G14">
+        <v>958</v>
+      </c>
+      <c r="H14">
+        <v>958</v>
+      </c>
+      <c r="I14">
+        <v>958</v>
+      </c>
+      <c r="J14">
+        <v>958</v>
+      </c>
+      <c r="K14">
+        <v>958</v>
       </c>
       <c r="M14">
         <v>958</v>
       </c>
+      <c r="N14">
+        <v>958</v>
+      </c>
+      <c r="O14">
+        <v>958</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>1222</v>
+      </c>
+      <c r="C15">
+        <v>1222</v>
+      </c>
+      <c r="D15">
+        <v>1222</v>
+      </c>
+      <c r="E15">
+        <v>1222</v>
+      </c>
+      <c r="F15">
+        <v>1222</v>
+      </c>
+      <c r="G15">
+        <v>1222</v>
+      </c>
+      <c r="H15">
+        <v>1222</v>
+      </c>
+      <c r="I15">
+        <v>1222</v>
+      </c>
+      <c r="J15">
+        <v>1222</v>
+      </c>
+      <c r="K15">
+        <v>1222</v>
       </c>
       <c r="M15">
         <v>1222</v>
       </c>
+      <c r="N15">
+        <v>1222</v>
+      </c>
+      <c r="O15">
+        <v>1222</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>1039</v>
+      </c>
+      <c r="C16">
+        <v>1039</v>
+      </c>
+      <c r="D16">
+        <v>1039</v>
+      </c>
+      <c r="E16">
+        <v>1039</v>
+      </c>
+      <c r="F16">
+        <v>1039</v>
+      </c>
+      <c r="G16">
+        <v>1039</v>
+      </c>
+      <c r="H16">
+        <v>1039</v>
+      </c>
+      <c r="I16">
+        <v>1039</v>
+      </c>
+      <c r="J16">
+        <v>1039</v>
+      </c>
+      <c r="K16">
+        <v>1039</v>
       </c>
       <c r="M16">
         <v>1039</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>1039</v>
+      </c>
+      <c r="O16">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>1150</v>
+      </c>
+      <c r="C17">
+        <v>1150</v>
+      </c>
+      <c r="D17">
+        <v>1150</v>
+      </c>
+      <c r="E17">
+        <v>1150</v>
+      </c>
+      <c r="F17">
+        <v>1150</v>
+      </c>
+      <c r="G17">
+        <v>1150</v>
+      </c>
+      <c r="H17">
+        <v>1150</v>
+      </c>
+      <c r="I17">
+        <v>1150</v>
+      </c>
+      <c r="J17">
+        <v>1150</v>
+      </c>
+      <c r="K17">
+        <v>1150</v>
       </c>
       <c r="M17">
         <v>1150</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>1150</v>
+      </c>
+      <c r="O17">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>1292</v>
+      </c>
+      <c r="C18">
+        <v>1292</v>
+      </c>
+      <c r="D18">
+        <v>1292</v>
+      </c>
+      <c r="E18">
+        <v>1292</v>
+      </c>
+      <c r="F18">
+        <v>1292</v>
+      </c>
+      <c r="G18">
+        <v>1292</v>
+      </c>
+      <c r="H18">
+        <v>1292</v>
+      </c>
+      <c r="I18">
+        <v>1292</v>
+      </c>
+      <c r="J18">
+        <v>1292</v>
+      </c>
+      <c r="K18">
+        <v>1292</v>
       </c>
       <c r="M18">
         <v>1292</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>1292</v>
+      </c>
+      <c r="O18">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>1221</v>
+      </c>
+      <c r="C19">
+        <v>1225</v>
+      </c>
+      <c r="D19">
+        <v>1235</v>
+      </c>
+      <c r="E19">
+        <v>1225</v>
+      </c>
+      <c r="F19">
+        <v>1246</v>
+      </c>
+      <c r="G19">
+        <v>1218</v>
+      </c>
+      <c r="H19">
+        <v>1243</v>
+      </c>
+      <c r="I19">
+        <v>1222</v>
+      </c>
+      <c r="J19">
+        <v>1230</v>
+      </c>
+      <c r="K19">
+        <v>1224</v>
       </c>
       <c r="M19">
         <v>1207</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>1218</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19:O40" si="1">AVERAGE(B19:K19)</f>
+        <v>1228.9000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>1001</v>
+      </c>
+      <c r="C20">
+        <v>992</v>
+      </c>
+      <c r="D20">
+        <v>995</v>
+      </c>
+      <c r="E20">
+        <v>1000</v>
+      </c>
+      <c r="F20">
+        <v>979</v>
+      </c>
+      <c r="G20">
+        <v>1000</v>
+      </c>
+      <c r="H20">
+        <v>979</v>
+      </c>
+      <c r="I20">
+        <v>1002</v>
+      </c>
+      <c r="J20">
+        <v>997</v>
+      </c>
+      <c r="K20">
+        <v>994</v>
       </c>
       <c r="M20">
         <v>945</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>979</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>993.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>821</v>
+      </c>
+      <c r="C21">
+        <v>797</v>
+      </c>
+      <c r="D21">
+        <v>802</v>
+      </c>
+      <c r="E21">
+        <v>793</v>
+      </c>
+      <c r="F21">
+        <v>793</v>
+      </c>
+      <c r="G21">
+        <v>819</v>
+      </c>
+      <c r="H21">
+        <v>807</v>
+      </c>
+      <c r="I21">
+        <v>821</v>
+      </c>
+      <c r="J21">
+        <v>816</v>
+      </c>
+      <c r="K21">
+        <v>823</v>
       </c>
       <c r="M21">
         <v>784</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>793</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>809.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>880</v>
+      </c>
+      <c r="C22">
+        <v>872</v>
+      </c>
+      <c r="D22">
+        <v>887</v>
+      </c>
+      <c r="E22">
+        <v>884</v>
+      </c>
+      <c r="F22">
+        <v>880</v>
+      </c>
+      <c r="G22">
+        <v>860</v>
+      </c>
+      <c r="H22">
+        <v>884</v>
+      </c>
+      <c r="I22">
+        <v>860</v>
+      </c>
+      <c r="J22">
+        <v>889</v>
+      </c>
+      <c r="K22">
+        <v>866</v>
       </c>
       <c r="M22">
         <v>848</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>860</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>876.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>877</v>
+      </c>
+      <c r="C23">
+        <v>893</v>
+      </c>
+      <c r="D23">
+        <v>877</v>
+      </c>
+      <c r="E23">
+        <v>890</v>
+      </c>
+      <c r="F23">
+        <v>875</v>
+      </c>
+      <c r="G23">
+        <v>892</v>
+      </c>
+      <c r="H23">
+        <v>871</v>
+      </c>
+      <c r="I23">
+        <v>879</v>
+      </c>
+      <c r="J23">
+        <v>875</v>
+      </c>
+      <c r="K23">
+        <v>891</v>
       </c>
       <c r="M23">
         <v>842</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>871</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>882</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>925</v>
+      </c>
+      <c r="C24">
+        <v>929</v>
+      </c>
+      <c r="D24">
+        <v>914</v>
+      </c>
+      <c r="E24">
+        <v>932</v>
+      </c>
+      <c r="F24">
+        <v>932</v>
+      </c>
+      <c r="G24">
+        <v>926</v>
+      </c>
+      <c r="H24">
+        <v>922</v>
+      </c>
+      <c r="I24">
+        <v>939</v>
+      </c>
+      <c r="J24">
+        <v>939</v>
+      </c>
+      <c r="K24">
+        <v>929</v>
       </c>
       <c r="M24">
         <v>902</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>914</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>928.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>1160</v>
+      </c>
+      <c r="C25">
+        <v>1141</v>
+      </c>
+      <c r="D25">
+        <v>1112</v>
+      </c>
+      <c r="E25">
+        <v>1174</v>
+      </c>
+      <c r="F25">
+        <v>1166</v>
+      </c>
+      <c r="G25">
+        <v>1174</v>
+      </c>
+      <c r="H25">
+        <v>1138</v>
+      </c>
+      <c r="I25">
+        <v>1174</v>
+      </c>
+      <c r="J25">
+        <v>1164</v>
+      </c>
+      <c r="K25">
+        <v>1154</v>
       </c>
       <c r="M25">
         <v>1046</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>1112</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>1155.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>1042</v>
+      </c>
+      <c r="C26">
+        <v>1024</v>
+      </c>
+      <c r="D26">
+        <v>1022</v>
+      </c>
+      <c r="E26">
+        <v>1069</v>
+      </c>
+      <c r="F26">
+        <v>1035</v>
+      </c>
+      <c r="G26">
+        <v>981</v>
+      </c>
+      <c r="H26">
+        <v>1044</v>
+      </c>
+      <c r="I26">
+        <v>1032</v>
+      </c>
+      <c r="J26">
+        <v>1013</v>
+      </c>
+      <c r="K26">
+        <v>1015</v>
       </c>
       <c r="M26">
         <v>927</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>981</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>1027.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>1051</v>
+      </c>
+      <c r="C27">
+        <v>1039</v>
+      </c>
+      <c r="D27">
+        <v>1045</v>
+      </c>
+      <c r="E27">
+        <v>1077</v>
+      </c>
+      <c r="F27">
+        <v>1074</v>
+      </c>
+      <c r="G27">
+        <v>1073</v>
+      </c>
+      <c r="H27">
+        <v>1039</v>
+      </c>
+      <c r="I27">
+        <v>1045</v>
+      </c>
+      <c r="J27">
+        <v>1049</v>
+      </c>
+      <c r="K27">
+        <v>1067</v>
       </c>
       <c r="M27">
         <v>1032</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>1039</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>1055.9000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>1031</v>
+      </c>
+      <c r="C28">
+        <v>1028</v>
+      </c>
+      <c r="D28">
+        <v>1026</v>
+      </c>
+      <c r="E28">
+        <v>1026</v>
+      </c>
+      <c r="F28">
+        <v>1015</v>
+      </c>
+      <c r="G28">
+        <v>1042</v>
+      </c>
+      <c r="H28">
+        <v>1022</v>
+      </c>
+      <c r="I28">
+        <v>1032</v>
+      </c>
+      <c r="J28">
+        <v>1021</v>
+      </c>
+      <c r="K28">
+        <v>1040</v>
       </c>
       <c r="M28">
         <v>935</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>1015</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>1028.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>1067</v>
+      </c>
+      <c r="C29">
+        <v>1046</v>
+      </c>
+      <c r="D29">
+        <v>1070</v>
+      </c>
+      <c r="E29">
+        <v>1072</v>
+      </c>
+      <c r="F29">
+        <v>1066</v>
+      </c>
+      <c r="G29">
+        <v>1061</v>
+      </c>
+      <c r="H29">
+        <v>1070</v>
+      </c>
+      <c r="I29">
+        <v>1073</v>
+      </c>
+      <c r="J29">
+        <v>1058</v>
+      </c>
+      <c r="K29">
+        <v>1067</v>
       </c>
       <c r="M29">
         <v>977</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>1046</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>1302</v>
+      </c>
+      <c r="C30">
+        <v>1288</v>
+      </c>
+      <c r="D30">
+        <v>1316</v>
+      </c>
+      <c r="E30">
+        <v>1320</v>
+      </c>
+      <c r="F30">
+        <v>1320</v>
+      </c>
+      <c r="G30">
+        <v>1302</v>
+      </c>
+      <c r="H30">
+        <v>1292</v>
+      </c>
+      <c r="I30">
+        <v>1289</v>
+      </c>
+      <c r="J30">
+        <v>1284</v>
+      </c>
+      <c r="K30">
+        <v>1291</v>
       </c>
       <c r="M30">
         <v>1218</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>1284</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>1300.4000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>1366</v>
+      </c>
+      <c r="C31">
+        <v>1345</v>
+      </c>
+      <c r="D31">
+        <v>1358</v>
+      </c>
+      <c r="E31">
+        <v>1369</v>
+      </c>
+      <c r="F31">
+        <v>1357</v>
+      </c>
+      <c r="G31">
+        <v>1379</v>
+      </c>
+      <c r="H31">
+        <v>1380</v>
+      </c>
+      <c r="I31">
+        <v>1371</v>
+      </c>
+      <c r="J31">
+        <v>1384</v>
+      </c>
+      <c r="K31">
+        <v>1338</v>
       </c>
       <c r="M31">
         <v>1235</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>1338</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>1364.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>1345</v>
+      </c>
+      <c r="C32">
+        <v>1346</v>
+      </c>
+      <c r="D32">
+        <v>1316</v>
+      </c>
+      <c r="E32">
+        <v>1352</v>
+      </c>
+      <c r="F32">
+        <v>1372</v>
+      </c>
+      <c r="G32">
+        <v>1343</v>
+      </c>
+      <c r="H32">
+        <v>1328</v>
+      </c>
+      <c r="I32">
+        <v>1363</v>
+      </c>
+      <c r="J32">
+        <v>1308</v>
+      </c>
+      <c r="K32">
+        <v>1366</v>
       </c>
       <c r="M32">
         <v>1216</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>1308</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>1343.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>1308</v>
+      </c>
+      <c r="C33">
+        <v>1321</v>
+      </c>
+      <c r="D33">
+        <v>1314</v>
+      </c>
+      <c r="E33">
+        <v>1303</v>
+      </c>
+      <c r="F33">
+        <v>1296</v>
+      </c>
+      <c r="G33">
+        <v>1306</v>
+      </c>
+      <c r="H33">
+        <v>1316</v>
+      </c>
+      <c r="I33">
+        <v>1317</v>
+      </c>
+      <c r="J33">
+        <v>1319</v>
+      </c>
+      <c r="K33">
+        <v>1332</v>
       </c>
       <c r="M33">
         <v>1152</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>1296</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>1313.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>1442</v>
+      </c>
+      <c r="C34">
+        <v>1416</v>
+      </c>
+      <c r="D34">
+        <v>1436</v>
+      </c>
+      <c r="E34">
+        <v>1422</v>
+      </c>
+      <c r="F34">
+        <v>1446</v>
+      </c>
+      <c r="G34">
+        <v>1452</v>
+      </c>
+      <c r="H34">
+        <v>1416</v>
+      </c>
+      <c r="I34">
+        <v>1449</v>
+      </c>
+      <c r="J34">
+        <v>1438</v>
+      </c>
+      <c r="K34">
+        <v>1425</v>
       </c>
       <c r="M34">
         <v>1355</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>1416</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>1434.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
       <c r="B35">
         <v>1784</v>
       </c>
+      <c r="C35">
+        <v>1784</v>
+      </c>
+      <c r="D35">
+        <v>1784</v>
+      </c>
+      <c r="E35">
+        <v>1784</v>
+      </c>
+      <c r="F35">
+        <v>1784</v>
+      </c>
+      <c r="G35">
+        <v>1784</v>
+      </c>
+      <c r="H35">
+        <v>1784</v>
+      </c>
+      <c r="I35">
+        <v>1784</v>
+      </c>
+      <c r="J35">
+        <v>1784</v>
+      </c>
+      <c r="K35">
+        <v>1784</v>
+      </c>
       <c r="M35">
         <v>1784</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>1784</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="1"/>
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>1858</v>
+      </c>
+      <c r="C36">
+        <v>1850</v>
+      </c>
+      <c r="D36">
+        <v>1861</v>
+      </c>
+      <c r="E36">
+        <v>1850</v>
+      </c>
+      <c r="F36">
+        <v>1856</v>
+      </c>
+      <c r="G36">
+        <v>1850</v>
+      </c>
+      <c r="H36">
+        <v>1865</v>
+      </c>
+      <c r="I36">
+        <v>1858</v>
+      </c>
+      <c r="J36">
+        <v>1850</v>
+      </c>
+      <c r="K36">
+        <v>1857</v>
       </c>
       <c r="M36">
         <v>1850</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>1850</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="1"/>
+        <v>1855.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>1721</v>
+      </c>
+      <c r="C37">
+        <v>1719</v>
+      </c>
+      <c r="D37">
+        <v>1719</v>
+      </c>
+      <c r="E37">
+        <v>1719</v>
+      </c>
+      <c r="F37">
+        <v>1725</v>
+      </c>
+      <c r="G37">
+        <v>1719</v>
+      </c>
+      <c r="H37">
+        <v>1719</v>
+      </c>
+      <c r="I37">
+        <v>1719</v>
+      </c>
+      <c r="J37">
+        <v>1719</v>
+      </c>
+      <c r="K37">
+        <v>1719</v>
       </c>
       <c r="M37">
         <v>1719</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>1719</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>1719.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>1782</v>
+      </c>
+      <c r="C38">
+        <v>1781</v>
+      </c>
+      <c r="D38">
+        <v>1773</v>
+      </c>
+      <c r="E38">
+        <v>1781</v>
+      </c>
+      <c r="F38">
+        <v>1780</v>
+      </c>
+      <c r="G38">
+        <v>1760</v>
+      </c>
+      <c r="H38">
+        <v>1746</v>
+      </c>
+      <c r="I38">
+        <v>1773</v>
+      </c>
+      <c r="J38">
+        <v>1801</v>
+      </c>
+      <c r="K38">
+        <v>1777</v>
       </c>
       <c r="M38">
         <v>1721</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>1746</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="1"/>
+        <v>1775.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>1902</v>
+      </c>
+      <c r="C39">
+        <v>1922</v>
+      </c>
+      <c r="D39">
+        <v>1907</v>
+      </c>
+      <c r="E39">
+        <v>1917</v>
+      </c>
+      <c r="F39">
+        <v>1892</v>
+      </c>
+      <c r="G39">
+        <v>1928</v>
+      </c>
+      <c r="H39">
+        <v>1888</v>
+      </c>
+      <c r="I39">
+        <v>1892</v>
+      </c>
+      <c r="J39">
+        <v>1893</v>
+      </c>
+      <c r="K39">
+        <v>1910</v>
       </c>
       <c r="M39">
         <v>1888</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>1888</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>1905.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40">
         <v>1337</v>
       </c>
+      <c r="C40">
+        <v>1385</v>
+      </c>
+      <c r="D40">
+        <v>1373</v>
+      </c>
+      <c r="E40">
+        <v>1366</v>
+      </c>
+      <c r="F40">
+        <v>1362</v>
+      </c>
+      <c r="G40">
+        <v>1380</v>
+      </c>
+      <c r="H40">
+        <v>1348</v>
+      </c>
+      <c r="I40">
+        <v>1356</v>
+      </c>
+      <c r="J40">
+        <v>1357</v>
+      </c>
+      <c r="K40">
+        <v>1375</v>
+      </c>
       <c r="M40">
         <v>1268</v>
+      </c>
+      <c r="N40">
+        <v>1337</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>1363.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>